<commit_message>
progressi in save load export
</commit_message>
<xml_diff>
--- a/resources/prova.xlsx
+++ b/resources/prova.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -23,7 +23,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>2023-07-07</t>
+    <t>2023-07-09</t>
   </si>
   <si>
     <t>10.0</t>
@@ -53,22 +53,22 @@
     <t>-10.0</t>
   </si>
   <si>
-    <t>2021-11-25</t>
-  </si>
-  <si>
-    <t>2022-01-28</t>
+    <t>2023-04-11</t>
+  </si>
+  <si>
+    <t>-10.67</t>
+  </si>
+  <si>
+    <t>2021-11-27</t>
+  </si>
+  <si>
+    <t>2022-01-30</t>
   </si>
   <si>
     <t>2001-09-13</t>
   </si>
   <si>
     <t>-13.0</t>
-  </si>
-  <si>
-    <t>2023-04-09</t>
-  </si>
-  <si>
-    <t>-10.67</t>
   </si>
 </sst>
 </file>
@@ -113,7 +113,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -212,21 +212,21 @@
         <v>3</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12">
@@ -234,32 +234,32 @@
         <v>3</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15">
@@ -267,21 +267,21 @@
         <v>3</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17">
@@ -289,15 +289,15 @@
         <v>3</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s" s="0">
         <v>4</v>
@@ -308,10 +308,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s" s="0">
         <v>7</v>
@@ -333,7 +333,7 @@
         <v>3</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C21" t="s" s="0">
         <v>5</v>
@@ -341,7 +341,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B22" t="s" s="0">
         <v>6</v>
@@ -355,10 +355,10 @@
         <v>3</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24">
@@ -366,10 +366,10 @@
         <v>3</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25">
@@ -377,10 +377,10 @@
         <v>3</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C25" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26">
@@ -388,32 +388,32 @@
         <v>3</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C26" t="s" s="0">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C27" t="s" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C28" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29">
@@ -421,10 +421,10 @@
         <v>3</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C29" t="s" s="0">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30">
@@ -432,21 +432,21 @@
         <v>3</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C30" t="s" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C31" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32">
@@ -454,32 +454,32 @@
         <v>3</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C32" t="s" s="0">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C33" t="s" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C34" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35">
@@ -487,21 +487,21 @@
         <v>3</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C35" t="s" s="0">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C36" t="s" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37">
@@ -509,15 +509,15 @@
         <v>3</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C37" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B38" t="s" s="0">
         <v>4</v>
@@ -528,10 +528,10 @@
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C39" t="s" s="0">
         <v>7</v>
@@ -553,7 +553,7 @@
         <v>3</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C41" t="s" s="0">
         <v>5</v>
@@ -561,7 +561,7 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B42" t="s" s="0">
         <v>6</v>
@@ -575,10 +575,10 @@
         <v>3</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C43" t="s" s="0">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44">
@@ -586,10 +586,10 @@
         <v>3</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C44" t="s" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45">
@@ -597,10 +597,10 @@
         <v>3</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C45" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46">
@@ -608,32 +608,32 @@
         <v>3</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C46" t="s" s="0">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C47" t="s" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C48" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49">
@@ -641,10 +641,10 @@
         <v>3</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C49" t="s" s="0">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50">
@@ -652,21 +652,21 @@
         <v>3</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C50" t="s" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C51" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52">
@@ -674,32 +674,32 @@
         <v>3</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C52" t="s" s="0">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C53" t="s" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C54" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55">
@@ -707,21 +707,21 @@
         <v>3</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C55" t="s" s="0">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C56" t="s" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57">
@@ -729,13 +729,68 @@
         <v>3</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C57" t="s" s="0">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="58"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B58" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C58" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B59" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="C59" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B60" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C60" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B61" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="C61" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B62" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C62" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>